<commit_message>
Add stress tests but remove from autotester
</commit_message>
<xml_diff>
--- a/AutomaticProjectTesting_Aug2015_VS2015/EmptyGeneralTesting/Release/Test16_Stress/ExcelQuery.xlsx
+++ b/AutomaticProjectTesting_Aug2015_VS2015/EmptyGeneralTesting/Release/Test16_Stress/ExcelQuery.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="632" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="632" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Next" sheetId="10" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="138">
   <si>
     <t>Index</t>
   </si>
@@ -271,6 +271,171 @@
   </si>
   <si>
     <t>Select &lt;s1, s2, s3&gt; such that Next*(s1, s2) and Next*(s2, s3)</t>
+  </si>
+  <si>
+    <t>Select a1 such that Affects(a1, a2)</t>
+  </si>
+  <si>
+    <t>assign a1,a2;</t>
+  </si>
+  <si>
+    <t>assign a1,a2,a3;</t>
+  </si>
+  <si>
+    <t>assign a1,a2,a3,a4;</t>
+  </si>
+  <si>
+    <t>assign a1,a2,a3,a4,a5;</t>
+  </si>
+  <si>
+    <t>assign a1,a2,a3,a4,a5,a6;</t>
+  </si>
+  <si>
+    <t>assign a1,a2,a3,a4,a5,a6,a7;</t>
+  </si>
+  <si>
+    <t>assign a1,a2,a3,a4,a5,a6,a7,a8;</t>
+  </si>
+  <si>
+    <t>assign a1,a2,a3,a4,a5,a6,a7,a8,a9;</t>
+  </si>
+  <si>
+    <t>assign a1,a2,a3,a4,a5,a6,a7,a8,a9,a10;</t>
+  </si>
+  <si>
+    <t>assign a1,a2,a3,a4,a5,a6,a7,a8,a9,a10,a11;</t>
+  </si>
+  <si>
+    <t>1Assign</t>
+  </si>
+  <si>
+    <t>2Assign</t>
+  </si>
+  <si>
+    <t>3Assign</t>
+  </si>
+  <si>
+    <t>4Assign</t>
+  </si>
+  <si>
+    <t>5Assign</t>
+  </si>
+  <si>
+    <t>6Assign</t>
+  </si>
+  <si>
+    <t>7Assign</t>
+  </si>
+  <si>
+    <t>8Assign</t>
+  </si>
+  <si>
+    <t>9Assign</t>
+  </si>
+  <si>
+    <t>10Assign</t>
+  </si>
+  <si>
+    <t>Select &lt;a1, a2&gt; such that Affects(a1, a2)</t>
+  </si>
+  <si>
+    <t>Select &lt;a1, a2, a3&gt; such that Affects(a1,a2) and Affects(a2, a3)</t>
+  </si>
+  <si>
+    <t>Select &lt;a1, a2, a3, a4&gt; such that Affects(a1,a2) and Affects(a2, a3) and Affects(a3, a4)</t>
+  </si>
+  <si>
+    <t>Select &lt;a1, a2, a3, a4, a5&gt; such that Affects(a1,a2) and Affects(a2, a3) and Affects(a3, a4) and Affects(a4, a5)</t>
+  </si>
+  <si>
+    <t>Select &lt;a1, a2, a3, a4, a5, a6&gt; such that Affects(a1,a2) and Affects(a2, a3) and Affects(a3, a4) and Affects(a4, a5) and Affects(a5, a6)</t>
+  </si>
+  <si>
+    <t>Select &lt;a1, a2, a3, a4, a5, a6, a7&gt; such that Affects(a1,a2) and Affects(a2, a3) and Affects(a3, a4) and Affects(a4, a5) and Affects(a5, a6) and Affects(a6, a7)</t>
+  </si>
+  <si>
+    <t>Select a2 such that Affects(a1, a2) and Affects(a2, a3)</t>
+  </si>
+  <si>
+    <t>Select a3 such that Affects(a1, a2) and Affects(a2, a3) and Affects(a3, a4)</t>
+  </si>
+  <si>
+    <t>Select a4 such that Affects(a1, a2) and Affects(a2, a3) and Affects(a3, a4) and Affects(a4,a5)</t>
+  </si>
+  <si>
+    <t>Select a5 such that Affects(a1, a2) and Affects(a2, a3) and Affects(a3, a4) and Affects(a4,a5) and Affects(a5, a6)</t>
+  </si>
+  <si>
+    <t>Select a6 such that Affects(a1, a2) and Affects(a2, a3) and Affects(a3, a4) and Affects(a4,a5) and Affects(a5, a6) and Affects(a6, a7)</t>
+  </si>
+  <si>
+    <t>Select a7 such that Affects(a1, a2) and Affects(a2, a3) and Affects(a3, a4) and Affects(a4,a5) and Affects(a5, a6) and Affects(a6, a7) and Affects(a7, a8)</t>
+  </si>
+  <si>
+    <t>Select a8 such that Affects(a1, a2) and Affects(a2, a3) and Affects(a3, a4) and Affects(a4,a5) and Affects(a5, a6) and Affects(a6, a7) and Affects(a7, a8) and Affects(a8, a9)</t>
+  </si>
+  <si>
+    <t>Select a9 such that Affects(a1, a2) and Affects(a2, a3) and Affects(a3, a4) and Affects(a4,a5) and Affects(a5, a6) and Affects(a6, a7) and Affects(a7, a8) and Affects(a8, a9) and Affects(a9, a10)</t>
+  </si>
+  <si>
+    <t>Select a10 such that Affects(a1, a2) and Affects(a2, a3) and Affects(a3, a4) and Affects(a4,a5) and Affects(a5, a6) and Affects(a6, a7) and Affects(a7, a8) and Affects(a8, a9) and Affects(a9, a10) and Affects(a10,a11)</t>
+  </si>
+  <si>
+    <t>assign a1, a2;</t>
+  </si>
+  <si>
+    <t>Select a1 such that Affects*(a1, a2)</t>
+  </si>
+  <si>
+    <t>Select a2 such that Affects*(a1, a2) and Affects*(a2, a3)</t>
+  </si>
+  <si>
+    <t>Select a3 such that Affects*(a1, a2) and Affects*(a2, a3) and Affects*(a3, a4)</t>
+  </si>
+  <si>
+    <t>Select &lt;a1, a2, a3&gt; such that Affects*(a1, a2) and Affects*(a2, a3)</t>
+  </si>
+  <si>
+    <t>Select &lt;a1,a2&gt; such that Affects*(a1, a2)</t>
+  </si>
+  <si>
+    <t>1AffectsStar</t>
+  </si>
+  <si>
+    <t>2AffectsStar</t>
+  </si>
+  <si>
+    <t>3AffectsStar</t>
+  </si>
+  <si>
+    <t>Select &lt;a1,a2,a3,a4&gt; such that Affects*(a1, a2) and Affects*(a2,a3) and Affects*(a3,a4)</t>
+  </si>
+  <si>
+    <t>1, 2, 3, 4, 5, 7, 8, 11, 12, 13, 14, 17, 25, 27, 28, 29, 30, 32, 38, 46, 47, 51, 52, 53, 54, 56, 57, 58, 59, 60, 61, 62, 63, 65, 67, 68, 71, 73, 74, 75, 82, 83, 85, 86, 87, 89, 91, 92, 95, 96, 97, 99, 103, 104, 106, 107, 108, 113, 116, 117, 118, 121, 122, 124, 125, 127, 128, 131, 134, 135, 136, 140, 141, 143, 144, 145, 147, 149, 150, 151, 153, 154, 156, 157, 158, 164, 165, 167, 189, 199, 217, 224, 225, 228, 230, 239, 242, 246, 250, 256, 260, 263, 266, 269</t>
+  </si>
+  <si>
+    <t>2, 3, 4, 7, 8, 12, 14, 17, 27, 30, 32, 46, 47, 52, 54, 56, 57, 59, 60, 61, 62, 63, 65, 67, 68, 75, 83, 85, 86, 87, 89, 91, 92, 95, 96, 97, 99, 107, 108, 113, 116, 117, 118, 121, 122, 124, 125, 127, 128, 131, 136, 140, 143, 144, 145, 147, 150, 151, 153, 154, 156, 158, 167, 246, 263</t>
+  </si>
+  <si>
+    <t>3, 7, 17, 30, 32, 46, 47, 54, 56, 57, 59, 60, 61, 62, 63, 65, 67, 68, 83, 85, 86, 87, 89, 91, 92, 95, 96, 97, 99, 108, 113, 116, 117, 118, 121, 122, 124, 125, 127, 128, 131, 143, 144, 145, 147, 151, 153, 154, 156, 158</t>
+  </si>
+  <si>
+    <t>7, 32, 46, 47, 54, 56, 57, 59, 60, 62, 63, 65, 67, 68, 83, 85, 86, 87, 89, 91, 92, 95, 96, 97, 99, 113, 116, 117, 118, 121, 122, 124, 125, 127, 128, 131, 143, 144, 145, 153, 154, 156, 158</t>
+  </si>
+  <si>
+    <t>46, 47, 54, 56, 57, 59, 60, 62, 63, 65, 67, 68, 83, 85, 86, 87, 89, 91, 92, 95, 96, 97, 99, 113, 116, 117, 118, 121, 122, 124, 125, 127, 128, 131, 143, 144, 145, 153, 154, 156, 158</t>
+  </si>
+  <si>
+    <t>1 2,1 4,1 7,1 8,1 9,103 100,103 83,103 93,104 107,106 108,106 113,106 118,106 119,106 128,106 132,107 108,107 113,107 116,107 117,107 119,107 121,107 124,107 128,107 129,107 131,107 132,108 113,108 125,108 132,11 12,113 114,116 113,116 118,116 119,116 128,116 132,117 113,117 125,117 132,118 119,12 20,121 113,121 118,121 122,121 125,121 127,122 124,124 125,124 127,125 122,125 128,127 122,128 113,128 116,128 117,128 119,128 121,128 124,128 128,128 129,128 131,128 132,13 14,13 17,131 113,131 125,131 132,134 140,135 136,135 137,136 137,14 17,14 18,14 35,14 36,140 147,141 143,143 144,144 143,144 145,145 143,147 148,149 150,150 151,150 153,150 154,150 159,151 153,151 159,153 156,154 154,154 156,154 158,156 153,156 158,156 159,157 156,157 158,158 153,158 154,158 159,164 167,165 167,167 168,17 18,17 20,189 190,199 201,199 205,199 209,199 210,2 3,217 223,224 226,225 226,228 229,230 233,239 241,242 246,246 247,25 27,250 253,250 255,256 259,260 263,260 265,263 265,266 268,269 271,27 30,27 31,27 32,27 34,28 30,28 31,28 34,29 31,29 32,29 33,29 34,3 7,30 31,30 32,30 33,30 34,32 33,38 39,4 7,46 47,46 67,46 68,47 46,47 54,47 67,47 68,47 69,5 6,5 9,51 52,52 61,52 68,53 62,54 56,54 57,54 60,56 59,57 62,57 63,57 65,57 68,58 46,58 54,58 61,58 67,58 68,58 69,59 60,60 67,60 68,61 62,62 46,62 47,62 56,62 57,62 60,62 63,62 67,62 68,62 69,63 46,63 47,63 62,63 68,63 69,65 66,67 62,67 63,67 65,67 68,68 69,7 9,71 100,71 72,71 83,71 85,71 91,71 92,73 100,73 85,73 87,73 97,74 75,74 86,74 89,74 90,74 92,74 95,74 99,75 100,75 83,75 93,8 9,82 100,82 83,82 93,83 85,83 86,85 87,86 80,86 83,86 86,86 89,86 90,86 92,87 80,87 89,89 91,89 99,91 100,92 93,92 95,92 96,92 97,92 99,95 100,96 95,97 99,99 100</t>
+  </si>
+  <si>
+    <t>1 2 3,1 4 7,1 7 9,1 8 9,103 83 85,103 83 86,104 107 108,104 107 113,104 107 116,104 107 117,104 107 119,104 107 121,104 107 124,104 107 128,104 107 129,104 107 131,104 107 132,106 108 113,106 108 125,106 108 132,106 113 114,106 118 119,106 128 113,106 128 116,106 128 117,106 128 119,106 128 121,106 128 124,106 128 128,106 128 129,106 128 131,106 128 132,107 108 113,107 108 125,107 108 132,107 113 114,107 116 113,107 116 118,107 116 119,107 116 128,107 116 132,107 117 113,107 117 125,107 117 132,107 121 113,107 121 118,107 121 122,107 121 125,107 121 127,107 124 125,107 124 127,107 128 113,107 128 116,107 128 117,107 128 119,107 128 121,107 128 124,107 128 128,107 128 129,107 128 131,107 128 132,107 131 113,107 131 125,107 131 132,108 113 114,108 125 122,108 125 128,11 12 20,116 113 114,116 118 119,116 128 113,116 128 116,116 128 117,116 128 119,116 128 121,116 128 124,116 128 128,116 128 129,116 128 131,116 128 132,117 113 114,117 125 122,117 125 128,121 113 114,121 118 119,121 122 124,121 125 122,121 125 128,121 127 122,122 124 125,122 124 127,124 125 122,124 125 128,124 127 122,125 122 124,125 128 113,125 128 116,125 128 117,125 128 119,125 128 121,125 128 124,125 128 128,125 128 129,125 128 131,125 128 132,127 122 124,128 113 114,128 116 113,128 116 118,128 116 119,128 116 128,128 116 132,128 117 113,128 117 125,128 117 132,128 121 113,128 121 118,128 121 122,128 121 125,128 121 127,128 124 125,128 124 127,128 128 113,128 128 116,128 128 117,128 128 119,128 128 121,128 128 124,128 128 128,128 128 129,128 128 131,128 128 132,128 131 113,128 131 125,128 131 132,13 14 17,13 14 18,13 14 35,13 14 36,13 17 18,13 17 20,131 113 114,131 125 122,131 125 128,134 140 147,135 136 137,14 17 18,14 17 20,140 147 148,141 143 144,143 144 143,143 144 145,144 143 144,144 145 143,145 143 144,149 150 151,149 150 153,149 150 154,149 150 159,150 151 153,150 151 159,150 153 156,150 154 154,150 154 156,150 154 158,151 153 156,153 156 153,153 156 158,153 156 159,154 154 154,154 154 156,154 154 158,154 156 153,154 156 158,154 156 159,154 158 153,154 158 154,154 158 159,156 153 156,156 158 153,156 158 154,156 158 159,157 156 153,157 156 158,157 156 159,157 158 153,157 158 154,157 158 159,158 153 156,158 154 154,158 154 156,158 154 158,164 167 168,165 167 168,2 3 7,242 246 247,25 27 30,25 27 31,25 27 32,25 27 34,260 263 265,27 30 31,27 30 32,27 30 33,27 30 34,27 32 33,28 30 31,28 30 32,28 30 33,28 30 34,29 32 33,3 7 9,30 32 33,4 7 9,46 47 46,46 47 54,46 47 67,46 47 68,46 47 69,46 67 62,46 67 63,46 67 65,46 67 68,46 68 69,47 46 47,47 46 67,47 46 68,47 54 56,47 54 57,47 54 60,47 67 62,47 67 63,47 67 65,47 67 68,47 68 69,51 52 61,51 52 68,52 61 62,52 68 69,53 62 46,53 62 47,53 62 56,53 62 57,53 62 60,53 62 63,53 62 67,53 62 68,53 62 69,54 56 59,54 57 62,54 57 63,54 57 65,54 57 68,54 60 67,54 60 68,56 59 60,57 62 46,57 62 47,57 62 56,57 62 57,57 62 60,57 62 63,57 62 67,57 62 68,57 62 69,57 63 46,57 63 47,57 63 62,57 63 68,57 63 69,57 65 66,57 68 69,58 46 47,58 46 67,58 46 68,58 54 56,58 54 57,58 54 60,58 61 62,58 67 62,58 67 63,58 67 65,58 67 68,58 68 69,59 60 67,59 60 68,60 67 62,60 67 63,60 67 65,60 67 68,60 68 69,61 62 46,61 62 47,61 62 56,61 62 57,61 62 60,61 62 63,61 62 67,61 62 68,61 62 69,62 46 47,62 46 67,62 46 68,62 47 46,62 47 54,62 47 67,62 47 68,62 47 69,62 56 59,62 57 62,62 57 63,62 57 65,62 57 68,62 60 67,62 60 68,62 63 46,62 63 47,62 63 62,62 63 68,62 63 69,62 67 62,62 67 63,62 67 65,62 67 68,62 68 69,63 46 47,63 46 67,63 46 68,63 47 46,63 47 54,63 47 67,63 47 68,63 47 69,63 62 46,63 62 47,63 62 56,63 62 57,63 62 60,63 62 63,63 62 67,63 62 68,63 62 69,63 68 69,67 62 46,67 62 47,67 62 56,67 62 57,67 62 60,67 62 63,67 62 67,67 62 68,67 62 69,67 63 46,67 63 47,67 63 62,67 63 68,67 63 69,67 65 66,67 68 69,71 83 85,71 83 86,71 85 87,71 91 100,71 92 93,71 92 95,71 92 96,71 92 97,71 92 99,73 85 87,73 87 80,73 87 89,73 97 99,74 75 100,74 75 83,74 75 93,74 86 80,74 86 83,74 86 86,74 86 89,74 86 90,74 86 92,74 89 91,74 89 99,74 92 93,74 92 95,74 92 96,74 92 97,74 92 99,74 95 100,74 99 100,75 83 85,75 83 86,82 83 85,82 83 86,83 85 87,83 86 80,83 86 83,83 86 86,83 86 89,83 86 90,83 86 92,85 87 80,85 87 89,86 83 85,86 83 86,86 86 80,86 86 83,86 86 86,86 86 89,86 86 90,86 86 92,86 89 91,86 89 99,86 92 93,86 92 95,86 92 96,86 92 97,86 92 99,87 89 91,87 89 99,89 91 100,89 99 100,92 95 100,92 96 95,92 97 99,92 99 100,96 95 100,97 99 100</t>
+  </si>
+  <si>
+    <t>1 2 3 7,1 4 7 9,103 83 85 87,103 83 86 80,103 83 86 83,103 83 86 86,103 83 86 89,103 83 86 90,103 83 86 92,104 107 108 113,104 107 108 125,104 107 108 132,104 107 113 114,104 107 116 113,104 107 116 118,104 107 116 119,104 107 116 128,104 107 116 132,104 107 117 113,104 107 117 125,104 107 117 132,104 107 121 113,104 107 121 118,104 107 121 122,104 107 121 125,104 107 121 127,104 107 124 125,104 107 124 127,104 107 128 113,104 107 128 116,104 107 128 117,104 107 128 119,104 107 128 121,104 107 128 124,104 107 128 128,104 107 128 129,104 107 128 131,104 107 128 132,104 107 131 113,104 107 131 125,104 107 131 132,106 108 113 114,106 108 125 122,106 108 125 128,106 128 113 114,106 128 116 113,106 128 116 118,106 128 116 119,106 128 116 128,106 128 116 132,106 128 117 113,106 128 117 125,106 128 117 132,106 128 121 113,106 128 121 118,106 128 121 122,106 128 121 125,106 128 121 127,106 128 124 125,106 128 124 127,106 128 128 113,106 128 128 116,106 128 128 117,106 128 128 119,106 128 128 121,106 128 128 124,106 128 128 128,106 128 128 129,106 128 128 131,106 128 128 132,106 128 131 113,106 128 131 125,106 128 131 132,107 108 113 114,107 108 125 122,107 108 125 128,107 116 113 114,107 116 118 119,107 116 128 113,107 116 128 116,107 116 128 117,107 116 128 119,107 116 128 121,107 116 128 124,107 116 128 128,107 116 128 129,107 116 128 131,107 116 128 132,107 117 113 114,107 117 125 122,107 117 125 128,107 121 113 114,107 121 118 119,107 121 122 124,107 121 125 122,107 121 125 128,107 121 127 122,107 124 125 122,107 124 125 128,107 124 127 122,107 128 113 114,107 128 116 113,107 128 116 118,107 128 116 119,107 128 116 128,107 128 116 132,107 128 117 113,107 128 117 125,107 128 117 132,107 128 121 113,107 128 121 118,107 128 121 122,107 128 121 125,107 128 121 127,107 128 124 125,107 128 124 127,107 128 128 113,107 128 128 116,107 128 128 117,107 128 128 119,107 128 128 121,107 128 128 124,107 128 128 128,107 128 128 129,107 128 128 131,107 128 128 132,107 128 131 113,107 128 131 125,107 128 131 132,107 131 113 114,107 131 125 122,107 131 125 128,108 125 122 124,108 125 128 113,108 125 128 116,108 125 128 117,108 125 128 119,108 125 128 121,108 125 128 124,108 125 128 128,108 125 128 129,108 125 128 131,108 125 128 132,116 128 113 114,116 128 116 113,116 128 116 118,116 128 116 119,116 128 116 128,116 128 116 132,116 128 117 113,116 128 117 125,116 128 117 132,116 128 121 113,116 128 121 118,116 128 121 122,116 128 121 125,116 128 121 127,116 128 124 125,116 128 124 127,116 128 128 113,116 128 128 116,116 128 128 117,116 128 128 119,116 128 128 121,116 128 128 124,116 128 128 128,116 128 128 129,116 128 128 131,116 128 128 132,116 128 131 113,116 128 131 125,116 128 131 132,117 125 122 124,117 125 128 113,117 125 128 116,117 125 128 117,117 125 128 119,117 125 128 121,117 125 128 124,117 125 128 128,117 125 128 129,117 125 128 131,117 125 128 132,121 122 124 125,121 122 124 127,121 125 122 124,121 125 128 113,121 125 128 116,121 125 128 117,121 125 128 119,121 125 128 121,121 125 128 124,121 125 128 128,121 125 128 129,121 125 128 131,121 125 128 132,121 127 122 124,122 124 125 122,122 124 125 128,122 124 127 122,124 125 122 124,124 125 128 113,124 125 128 116,124 125 128 117,124 125 128 119,124 125 128 121,124 125 128 124,124 125 128 128,124 125 128 129,124 125 128 131,124 125 128 132,124 127 122 124,125 122 124 125,125 122 124 127,125 128 113 114,125 128 116 113,125 128 116 118,125 128 116 119,125 128 116 128,125 128 116 132,125 128 117 113,125 128 117 125,125 128 117 132,125 128 121 113,125 128 121 118,125 128 121 122,125 128 121 125,125 128 121 127,125 128 124 125,125 128 124 127,125 128 128 113,125 128 128 116,125 128 128 117,125 128 128 119,125 128 128 121,125 128 128 124,125 128 128 128,125 128 128 129,125 128 128 131,125 128 128 132,125 128 131 113,125 128 131 125,125 128 131 132,127 122 124 125,127 122 124 127,128 116 113 114,128 116 118 119,128 116 128 113,128 116 128 116,128 116 128 117,128 116 128 119,128 116 128 121,128 116 128 124,128 116 128 128,128 116 128 129,128 116 128 131,128 116 128 132,128 117 113 114,128 117 125 122,128 117 125 128,128 121 113 114,128 121 118 119,128 121 122 124,128 121 125 122,128 121 125 128,128 121 127 122,128 124 125 122,128 124 125 128,128 124 127 122,128 128 113 114,128 128 116 113,128 128 116 118,128 128 116 119,128 128 116 128,128 128 116 132,128 128 117 113,128 128 117 125,128 128 117 132,128 128 121 113,128 128 121 118,128 128 121 122,128 128 121 125,128 128 121 127,128 128 124 125,128 128 124 127,128 128 128 113,128 128 128 116,128 128 128 117,128 128 128 119,128 128 128 121,128 128 128 124,128 128 128 128,128 128 128 129,128 128 128 131,128 128 128 132,128 128 131 113,128 128 131 125,128 128 131 132,128 131 113 114,128 131 125 122,128 131 125 128,13 14 17 18,13 14 17 20,131 125 122 124,131 125 128 113,131 125 128 116,131 125 128 117,131 125 128 119,131 125 128 121,131 125 128 124,131 125 128 128,131 125 128 129,131 125 128 131,131 125 128 132,134 140 147 148,141 143 144 143,141 143 144 145,143 144 143 144,143 144 145 143,144 143 144 143,144 143 144 145,144 145 143 144,145 143 144 143,145 143 144 145,149 150 151 153,149 150 151 159,149 150 153 156,149 150 154 154,149 150 154 156,149 150 154 158,150 151 153 156,150 153 156 153,150 153 156 158,150 153 156 159,150 154 154 154,150 154 154 156,150 154 154 158,150 154 156 153,150 154 156 158,150 154 156 159,150 154 158 153,150 154 158 154,150 154 158 159,151 153 156 153,151 153 156 158,151 153 156 159,153 156 153 156,153 156 158 153,153 156 158 154,153 156 158 159,154 154 154 154,154 154 154 156,154 154 154 158,154 154 156 153,154 154 156 158,154 154 156 159,154 154 158 153,154 154 158 154,154 154 158 159,154 156 153 156,154 156 158 153,154 156 158 154,154 156 158 159,154 158 153 156,154 158 154 154,154 158 154 156,154 158 154 158,156 153 156 153,156 153 156 158,156 153 156 159,156 158 153 156,156 158 154 154,156 158 154 156,156 158 154 158,157 156 153 156,157 156 158 153,157 156 158 154,157 156 158 159,157 158 153 156,157 158 154 154,157 158 154 156,157 158 154 158,158 153 156 153,158 153 156 158,158 153 156 159,158 154 154 154,158 154 154 156,158 154 154 158,158 154 156 153,158 154 156 158,158 154 156 159,158 154 158 153,158 154 158 154,158 154 158 159,2 3 7 9,25 27 30 31,25 27 30 32,25 27 30 33,25 27 30 34,25 27 32 33,27 30 32 33,28 30 32 33,46 47 46 47,46 47 46 67,46 47 46 68,46 47 54 56,46 47 54 57,46 47 54 60,46 47 67 62,46 47 67 63,46 47 67 65,46 47 67 68,46 47 68 69,46 67 62 46,46 67 62 47,46 67 62 56,46 67 62 57,46 67 62 60,46 67 62 63,46 67 62 67,46 67 62 68,46 67 62 69,46 67 63 46,46 67 63 47,46 67 63 62,46 67 63 68,46 67 63 69,46 67 65 66,46 67 68 69,47 46 47 46,47 46 47 54,47 46 47 67,47 46 47 68,47 46 47 69,47 46 67 62,47 46 67 63,47 46 67 65,47 46 67 68,47 46 68 69,47 54 56 59,47 54 57 62,47 54 57 63,47 54 57 65,47 54 57 68,47 54 60 67,47 54 60 68,47 67 62 46,47 67 62 47,47 67 62 56,47 67 62 57,47 67 62 60,47 67 62 63,47 67 62 67,47 67 62 68,47 67 62 69,47 67 63 46,47 67 63 47,47 67 63 62,47 67 63 68,47 67 63 69,47 67 65 66,47 67 68 69,51 52 61 62,51 52 68 69,52 61 62 46,52 61 62 47,52 61 62 56,52 61 62 57,52 61 62 60,52 61 62 63,52 61 62 67,52 61 62 68,52 61 62 69,53 62 46 47,53 62 46 67,53 62 46 68,53 62 47 46,53 62 47 54,53 62 47 67,53 62 47 68,53 62 47 69,53 62 56 59,53 62 57 62,53 62 57 63,53 62 57 65,53 62 57 68,53 62 60 67,53 62 60 68,53 62 63 46,53 62 63 47,53 62 63 62,53 62 63 68,53 62 63 69,53 62 67 62,53 62 67 63,53 62 67 65,53 62 67 68,53 62 68 69,54 56 59 60,54 57 62 46,54 57 62 47,54 57 62 56,54 57 62 57,54 57 62 60,54 57 62 63,54 57 62 67,54 57 62 68,54 57 62 69,54 57 63 46,54 57 63 47,54 57 63 62,54 57 63 68,54 57 63 69,54 57 65 66,54 57 68 69,54 60 67 62,54 60 67 63,54 60 67 65,54 60 67 68,54 60 68 69,56 59 60 67,56 59 60 68,57 62 46 47,57 62 46 67,57 62 46 68,57 62 47 46,57 62 47 54,57 62 47 67,57 62 47 68,57 62 47 69,57 62 56 59,57 62 57 62,57 62 57 63,57 62 57 65,57 62 57 68,57 62 60 67,57 62 60 68,57 62 63 46,57 62 63 47,57 62 63 62,57 62 63 68,57 62 63 69,57 62 67 62,57 62 67 63,57 62 67 65,57 62 67 68,57 62 68 69,57 63 46 47,57 63 46 67,57 63 46 68,57 63 47 46,57 63 47 54,57 63 47 67,57 63 47 68,57 63 47 69,57 63 62 46,57 63 62 47,57 63 62 56,57 63 62 57,57 63 62 60,57 63 62 63,57 63 62 67,57 63 62 68,57 63 62 69,57 63 68 69,58 46 47 46,58 46 47 54,58 46 47 67,58 46 47 68,58 46 47 69,58 46 67 62,58 46 67 63,58 46 67 65,58 46 67 68,58 46 68 69,58 54 56 59,58 54 57 62,58 54 57 63,58 54 57 65,58 54 57 68,58 54 60 67,58 54 60 68,58 61 62 46,58 61 62 47,58 61 62 56,58 61 62 57,58 61 62 60,58 61 62 63,58 61 62 67,58 61 62 68,58 61 62 69,58 67 62 46,58 67 62 47,58 67 62 56,58 67 62 57,58 67 62 60,58 67 62 63,58 67 62 67,58 67 62 68,58 67 62 69,58 67 63 46,58 67 63 47,58 67 63 62,58 67 63 68,58 67 63 69,58 67 65 66,58 67 68 69,59 60 67 62,59 60 67 63,59 60 67 65,59 60 67 68,59 60 68 69,60 67 62 46,60 67 62 47,60 67 62 56,60 67 62 57,60 67 62 60,60 67 62 63,60 67 62 67,60 67 62 68,60 67 62 69,60 67 63 46,60 67 63 47,60 67 63 62,60 67 63 68,60 67 63 69,60 67 65 66,60 67 68 69,61 62 46 47,61 62 46 67,61 62 46 68,61 62 47 46,61 62 47 54,61 62 47 67,61 62 47 68,61 62 47 69,61 62 56 59,61 62 57 62,61 62 57 63,61 62 57 65,61 62 57 68,61 62 60 67,61 62 60 68,61 62 63 46,61 62 63 47,61 62 63 62,61 62 63 68,61 62 63 69,61 62 67 62,61 62 67 63,61 62 67 65,61 62 67 68,61 62 68 69,62 46 47 46,62 46 47 54,62 46 47 67,62 46 47 68,62 46 47 69,62 46 67 62,62 46 67 63,62 46 67 65,62 46 67 68,62 46 68 69,62 47 46 47,62 47 46 67,62 47 46 68,62 47 54 56,62 47 54 57,62 47 54 60,62 47 67 62,62 47 67 63,62 47 67 65,62 47 67 68,62 47 68 69,62 56 59 60,62 57 62 46,62 57 62 47,62 57 62 56,62 57 62 57,62 57 62 60,62 57 62 63,62 57 62 67,62 57 62 68,62 57 62 69,62 57 63 46,62 57 63 47,62 57 63 62,62 57 63 68,62 57 63 69,62 57 65 66,62 57 68 69,62 60 67 62,62 60 67 63,62 60 67 65,62 60 67 68,62 60 68 69,62 63 46 47,62 63 46 67,62 63 46 68,62 63 47 46,62 63 47 54,62 63 47 67,62 63 47 68,62 63 47 69,62 63 62 46,62 63 62 47,62 63 62 56,62 63 62 57,62 63 62 60,62 63 62 63,62 63 62 67,62 63 62 68,62 63 62 69,62 63 68 69,62 67 62 46,62 67 62 47,62 67 62 56,62 67 62 57,62 67 62 60,62 67 62 63,62 67 62 67,62 67 62 68,62 67 62 69,62 67 63 46,62 67 63 47,62 67 63 62,62 67 63 68,62 67 63 69,62 67 65 66,62 67 68 69,63 46 47 46,63 46 47 54,63 46 47 67,63 46 47 68,63 46 47 69,63 46 67 62,63 46 67 63,63 46 67 65,63 46 67 68,63 46 68 69,63 47 46 47,63 47 46 67,63 47 46 68,63 47 54 56,63 47 54 57,63 47 54 60,63 47 67 62,63 47 67 63,63 47 67 65,63 47 67 68,63 47 68 69,63 62 46 47,63 62 46 67,63 62 46 68,63 62 47 46,63 62 47 54,63 62 47 67,63 62 47 68,63 62 47 69,63 62 56 59,63 62 57 62,63 62 57 63,63 62 57 65,63 62 57 68,63 62 60 67,63 62 60 68,63 62 63 46,63 62 63 47,63 62 63 62,63 62 63 68,63 62 63 69,63 62 67 62,63 62 67 63,63 62 67 65,63 62 67 68,63 62 68 69,67 62 46 47,67 62 46 67,67 62 46 68,67 62 47 46,67 62 47 54,67 62 47 67,67 62 47 68,67 62 47 69,67 62 56 59,67 62 57 62,67 62 57 63,67 62 57 65,67 62 57 68,67 62 60 67,67 62 60 68,67 62 63 46,67 62 63 47,67 62 63 62,67 62 63 68,67 62 63 69,67 62 67 62,67 62 67 63,67 62 67 65,67 62 67 68,67 62 68 69,67 63 46 47,67 63 46 67,67 63 46 68,67 63 47 46,67 63 47 54,67 63 47 67,67 63 47 68,67 63 47 69,67 63 62 46,67 63 62 47,67 63 62 56,67 63 62 57,67 63 62 60,67 63 62 63,67 63 62 67,67 63 62 68,67 63 62 69,67 63 68 69,71 83 85 87,71 83 86 80,71 83 86 83,71 83 86 86,71 83 86 89,71 83 86 90,71 83 86 92,71 85 87 80,71 85 87 89,71 92 95 100,71 92 96 95,71 92 97 99,71 92 99 100,73 85 87 80,73 85 87 89,73 87 89 91,73 87 89 99,73 97 99 100,74 75 83 85,74 75 83 86,74 86 83 85,74 86 83 86,74 86 86 80,74 86 86 83,74 86 86 86,74 86 86 89,74 86 86 90,74 86 86 92,74 86 89 91,74 86 89 99,74 86 92 93,74 86 92 95,74 86 92 96,74 86 92 97,74 86 92 99,74 89 91 100,74 89 99 100,74 92 95 100,74 92 96 95,74 92 97 99,74 92 99 100,75 83 85 87,75 83 86 80,75 83 86 83,75 83 86 86,75 83 86 89,75 83 86 90,75 83 86 92,82 83 85 87,82 83 86 80,82 83 86 83,82 83 86 86,82 83 86 89,82 83 86 90,82 83 86 92,83 85 87 80,83 85 87 89,83 86 83 85,83 86 83 86,83 86 86 80,83 86 86 83,83 86 86 86,83 86 86 89,83 86 86 90,83 86 86 92,83 86 89 91,83 86 89 99,83 86 92 93,83 86 92 95,83 86 92 96,83 86 92 97,83 86 92 99,85 87 89 91,85 87 89 99,86 83 85 87,86 83 86 80,86 83 86 83,86 83 86 86,86 83 86 89,86 83 86 90,86 83 86 92,86 86 83 85,86 86 83 86,86 86 86 80,86 86 86 83,86 86 86 86,86 86 86 89,86 86 86 90,86 86 86 92,86 86 89 91,86 86 89 99,86 86 92 93,86 86 92 95,86 86 92 96,86 86 92 97,86 86 92 99,86 89 91 100,86 89 99 100,86 92 95 100,86 92 96 95,86 92 97 99,86 92 99 100,87 89 91 100,87 89 99 100,92 96 95 100,92 97 99 100</t>
+  </si>
+  <si>
+    <t>1 2,1 3,1 4,1 7,1 8,1 9,103 100,103 80,103 83,103 85,103 86,103 87,103 89,103 90,103 91,103 92,103 93,103 95,103 96,103 97,103 99,104 107,104 108,104 113,104 114,104 116,104 117,104 118,104 119,104 121,104 122,104 124,104 125,104 127,104 128,104 129,104 131,104 132,106 108,106 113,106 114,106 116,106 117,106 118,106 119,106 121,106 122,106 124,106 125,106 127,106 128,106 129,106 131,106 132,107 108,107 113,107 114,107 116,107 117,107 118,107 119,107 121,107 122,107 124,107 125,107 127,107 128,107 129,107 131,107 132,108 113,108 114,108 116,108 117,108 118,108 119,108 121,108 122,108 124,108 125,108 127,108 128,108 129,108 131,108 132,11 12,11 20,113 114,116 113,116 114,116 116,116 117,116 118,116 119,116 121,116 122,116 124,116 125,116 127,116 128,116 129,116 131,116 132,117 113,117 114,117 116,117 117,117 118,117 119,117 121,117 122,117 124,117 125,117 127,117 128,117 129,117 131,117 132,118 119,12 20,121 113,121 114,121 116,121 117,121 118,121 119,121 121,121 122,121 124,121 125,121 127,121 128,121 129,121 131,121 132,122 113,122 114,122 116,122 117,122 118,122 119,122 121,122 122,122 124,122 125,122 127,122 128,122 129,122 131,122 132,124 113,124 114,124 116,124 117,124 118,124 119,124 121,124 122,124 124,124 125,124 127,124 128,124 129,124 131,124 132,125 113,125 114,125 116,125 117,125 118,125 119,125 121,125 122,125 124,125 125,125 127,125 128,125 129,125 131,125 132,127 113,127 114,127 116,127 117,127 118,127 119,127 121,127 122,127 124,127 125,127 127,127 128,127 129,127 131,127 132,128 113,128 114,128 116,128 117,128 118,128 119,128 121,128 122,128 124,128 125,128 127,128 128,128 129,128 131,128 132,13 14,13 17,13 18,13 20,13 35,13 36,131 113,131 114,131 116,131 117,131 118,131 119,131 121,131 122,131 124,131 125,131 127,131 128,131 129,131 131,131 132,134 140,134 147,134 148,135 136,135 137,136 137,14 17,14 18,14 20,14 35,14 36,140 147,140 148,141 143,141 144,141 145,143 143,143 144,143 145,144 143,144 144,144 145,145 143,145 144,145 145,147 148,149 150,149 151,149 153,149 154,149 156,149 158,149 159,150 151,150 153,150 154,150 156,150 158,150 159,151 153,151 154,151 156,151 158,151 159,153 153,153 154,153 156,153 158,153 159,154 153,154 154,154 156,154 158,154 159,156 153,156 154,156 156,156 158,156 159,157 153,157 154,157 156,157 158,157 159,158 153,158 154,158 156,158 158,158 159,164 167,164 168,165 167,165 168,167 168,17 18,17 20,189 190,199 201,199 205,199 209,199 210,2 3,2 7,2 9,217 223,224 226,225 226,228 229,230 233,239 241,242 246,242 247,246 247,25 27,25 30,25 31,25 32,25 33,25 34,250 253,250 255,256 259,260 263,260 265,263 265,266 268,269 271,27 30,27 31,27 32,27 33,27 34,28 30,28 31,28 32,28 33,28 34,29 31,29 32,29 33,29 34,3 7,3 9,30 31,30 32,30 33,30 34,32 33,38 39,4 7,4 9,46 46,46 47,46 54,46 56,46 57,46 59,46 60,46 62,46 63,46 65,46 66,46 67,46 68,46 69,47 46,47 47,47 54,47 56,47 57,47 59,47 60,47 62,47 63,47 65,47 66,47 67,47 68,47 69,5 6,5 9,51 46,51 47,51 52,51 54,51 56,51 57,51 59,51 60,51 61,51 62,51 63,51 65,51 66,51 67,51 68,51 69,52 46,52 47,52 54,52 56,52 57,52 59,52 60,52 61,52 62,52 63,52 65,52 66,52 67,52 68,52 69,53 46,53 47,53 54,53 56,53 57,53 59,53 60,53 62,53 63,53 65,53 66,53 67,53 68,53 69,54 46,54 47,54 54,54 56,54 57,54 59,54 60,54 62,54 63,54 65,54 66,54 67,54 68,54 69,56 46,56 47,56 54,56 56,56 57,56 59,56 60,56 62,56 63,56 65,56 66,56 67,56 68,56 69,57 46,57 47,57 54,57 56,57 57,57 59,57 60,57 62,57 63,57 65,57 66,57 67,57 68,57 69,58 46,58 47,58 54,58 56,58 57,58 59,58 60,58 61,58 62,58 63,58 65,58 66,58 67,58 68,58 69,59 46,59 47,59 54,59 56,59 57,59 59,59 60,59 62,59 63,59 65,59 66,59 67,59 68,59 69,60 46,60 47,60 54,60 56,60 57,60 59,60 60,60 62,60 63,60 65,60 66,60 67,60 68,60 69,61 46,61 47,61 54,61 56,61 57,61 59,61 60,61 62,61 63,61 65,61 66,61 67,61 68,61 69,62 46,62 47,62 54,62 56,62 57,62 59,62 60,62 62,62 63,62 65,62 66,62 67,62 68,62 69,63 46,63 47,63 54,63 56,63 57,63 59,63 60,63 62,63 63,63 65,63 66,63 67,63 68,63 69,65 66,67 46,67 47,67 54,67 56,67 57,67 59,67 60,67 62,67 63,67 65,67 66,67 67,67 68,67 69,68 69,7 9,71 100,71 72,71 80,71 83,71 85,71 86,71 87,71 89,71 90,71 91,71 92,71 93,71 95,71 96,71 97,71 99,73 100,73 80,73 85,73 87,73 89,73 91,73 97,73 99,74 100,74 75,74 80,74 83,74 85,74 86,74 87,74 89,74 90,74 91,74 92,74 93,74 95,74 96,74 97,74 99,75 100,75 80,75 83,75 85,75 86,75 87,75 89,75 90,75 91,75 92,75 93,75 95,75 96,75 97,75 99,8 9,82 100,82 80,82 83,82 85,82 86,82 87,82 89,82 90,82 91,82 92,82 93,82 95,82 96,82 97,82 99,83 100,83 80,83 83,83 85,83 86,83 87,83 89,83 90,83 91,83 92,83 93,83 95,83 96,83 97,83 99,85 100,85 80,85 87,85 89,85 91,85 99,86 100,86 80,86 83,86 85,86 86,86 87,86 89,86 90,86 91,86 92,86 93,86 95,86 96,86 97,86 99,87 100,87 80,87 89,87 91,87 99,89 100,89 91,89 99,91 100,92 100,92 93,92 95,92 96,92 97,92 99,95 100,96 100,96 95,97 100,97 99,99 100</t>
   </si>
 </sst>
 </file>
@@ -375,7 +540,103 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="26">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF57BB8A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE67C73"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF57BB8A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE67C73"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF57BB8A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE67C73"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF57BB8A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE67C73"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -876,8 +1137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC3F969A-AF06-4B88-BDEC-BD9AE21F1F8A}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1339,34 +1600,34 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:G23 G25:G1048576">
-    <cfRule type="cellIs" dxfId="17" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="13" operator="equal">
       <formula>"BUG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="14" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G22:G23">
-    <cfRule type="cellIs" dxfId="15" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="9" operator="equal">
       <formula>"BUG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="10" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G24">
-    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="7" operator="equal">
       <formula>"BUG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="8" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G24">
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="5" operator="equal">
       <formula>"BUG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="6" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1377,17 +1638,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDD5F34A-C32F-4F9E-A4EF-99404DBA2DE9}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD120"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="42.28515625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="200.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40.42578125" style="5" customWidth="1"/>
     <col min="5" max="5" width="87.5703125" style="4" customWidth="1"/>
     <col min="6" max="6" width="47.28515625" style="4" customWidth="1"/>
@@ -1418,8 +1679,407 @@
         <v>6</v>
       </c>
     </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>13</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>14</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>15</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>16</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>17</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+    </row>
+    <row r="19" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>18</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+    </row>
+    <row r="20" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>19</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+    </row>
+    <row r="21" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>20</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>21</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>22</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="G1:G1048576">
+  <conditionalFormatting sqref="G1:G17 G23:G1048576">
+    <cfRule type="cellIs" dxfId="17" priority="9" operator="equal">
+      <formula>"BUG"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="10" operator="equal">
+      <formula>"PASS"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G18:G19 G22">
+    <cfRule type="cellIs" dxfId="15" priority="7" operator="equal">
+      <formula>"BUG"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="8" operator="equal">
+      <formula>"PASS"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G18:G19">
+    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
+      <formula>"BUG"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
+      <formula>"PASS"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G20:G21">
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
+      <formula>"BUG"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
+      <formula>"PASS"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G20:G21">
     <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>"BUG"</formula>
     </cfRule>
@@ -1428,6 +2088,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add Andy stress test in test16
</commit_message>
<xml_diff>
--- a/AutomaticProjectTesting_Aug2015_VS2015/EmptyGeneralTesting/Release/Test16_Stress/ExcelQuery.xlsx
+++ b/AutomaticProjectTesting_Aug2015_VS2015/EmptyGeneralTesting/Release/Test16_Stress/ExcelQuery.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="632" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="632" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Next" sheetId="10" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="179">
   <si>
     <t>Index</t>
   </si>
@@ -436,6 +436,129 @@
   </si>
   <si>
     <t>1 2,1 3,1 4,1 7,1 8,1 9,103 100,103 80,103 83,103 85,103 86,103 87,103 89,103 90,103 91,103 92,103 93,103 95,103 96,103 97,103 99,104 107,104 108,104 113,104 114,104 116,104 117,104 118,104 119,104 121,104 122,104 124,104 125,104 127,104 128,104 129,104 131,104 132,106 108,106 113,106 114,106 116,106 117,106 118,106 119,106 121,106 122,106 124,106 125,106 127,106 128,106 129,106 131,106 132,107 108,107 113,107 114,107 116,107 117,107 118,107 119,107 121,107 122,107 124,107 125,107 127,107 128,107 129,107 131,107 132,108 113,108 114,108 116,108 117,108 118,108 119,108 121,108 122,108 124,108 125,108 127,108 128,108 129,108 131,108 132,11 12,11 20,113 114,116 113,116 114,116 116,116 117,116 118,116 119,116 121,116 122,116 124,116 125,116 127,116 128,116 129,116 131,116 132,117 113,117 114,117 116,117 117,117 118,117 119,117 121,117 122,117 124,117 125,117 127,117 128,117 129,117 131,117 132,118 119,12 20,121 113,121 114,121 116,121 117,121 118,121 119,121 121,121 122,121 124,121 125,121 127,121 128,121 129,121 131,121 132,122 113,122 114,122 116,122 117,122 118,122 119,122 121,122 122,122 124,122 125,122 127,122 128,122 129,122 131,122 132,124 113,124 114,124 116,124 117,124 118,124 119,124 121,124 122,124 124,124 125,124 127,124 128,124 129,124 131,124 132,125 113,125 114,125 116,125 117,125 118,125 119,125 121,125 122,125 124,125 125,125 127,125 128,125 129,125 131,125 132,127 113,127 114,127 116,127 117,127 118,127 119,127 121,127 122,127 124,127 125,127 127,127 128,127 129,127 131,127 132,128 113,128 114,128 116,128 117,128 118,128 119,128 121,128 122,128 124,128 125,128 127,128 128,128 129,128 131,128 132,13 14,13 17,13 18,13 20,13 35,13 36,131 113,131 114,131 116,131 117,131 118,131 119,131 121,131 122,131 124,131 125,131 127,131 128,131 129,131 131,131 132,134 140,134 147,134 148,135 136,135 137,136 137,14 17,14 18,14 20,14 35,14 36,140 147,140 148,141 143,141 144,141 145,143 143,143 144,143 145,144 143,144 144,144 145,145 143,145 144,145 145,147 148,149 150,149 151,149 153,149 154,149 156,149 158,149 159,150 151,150 153,150 154,150 156,150 158,150 159,151 153,151 154,151 156,151 158,151 159,153 153,153 154,153 156,153 158,153 159,154 153,154 154,154 156,154 158,154 159,156 153,156 154,156 156,156 158,156 159,157 153,157 154,157 156,157 158,157 159,158 153,158 154,158 156,158 158,158 159,164 167,164 168,165 167,165 168,167 168,17 18,17 20,189 190,199 201,199 205,199 209,199 210,2 3,2 7,2 9,217 223,224 226,225 226,228 229,230 233,239 241,242 246,242 247,246 247,25 27,25 30,25 31,25 32,25 33,25 34,250 253,250 255,256 259,260 263,260 265,263 265,266 268,269 271,27 30,27 31,27 32,27 33,27 34,28 30,28 31,28 32,28 33,28 34,29 31,29 32,29 33,29 34,3 7,3 9,30 31,30 32,30 33,30 34,32 33,38 39,4 7,4 9,46 46,46 47,46 54,46 56,46 57,46 59,46 60,46 62,46 63,46 65,46 66,46 67,46 68,46 69,47 46,47 47,47 54,47 56,47 57,47 59,47 60,47 62,47 63,47 65,47 66,47 67,47 68,47 69,5 6,5 9,51 46,51 47,51 52,51 54,51 56,51 57,51 59,51 60,51 61,51 62,51 63,51 65,51 66,51 67,51 68,51 69,52 46,52 47,52 54,52 56,52 57,52 59,52 60,52 61,52 62,52 63,52 65,52 66,52 67,52 68,52 69,53 46,53 47,53 54,53 56,53 57,53 59,53 60,53 62,53 63,53 65,53 66,53 67,53 68,53 69,54 46,54 47,54 54,54 56,54 57,54 59,54 60,54 62,54 63,54 65,54 66,54 67,54 68,54 69,56 46,56 47,56 54,56 56,56 57,56 59,56 60,56 62,56 63,56 65,56 66,56 67,56 68,56 69,57 46,57 47,57 54,57 56,57 57,57 59,57 60,57 62,57 63,57 65,57 66,57 67,57 68,57 69,58 46,58 47,58 54,58 56,58 57,58 59,58 60,58 61,58 62,58 63,58 65,58 66,58 67,58 68,58 69,59 46,59 47,59 54,59 56,59 57,59 59,59 60,59 62,59 63,59 65,59 66,59 67,59 68,59 69,60 46,60 47,60 54,60 56,60 57,60 59,60 60,60 62,60 63,60 65,60 66,60 67,60 68,60 69,61 46,61 47,61 54,61 56,61 57,61 59,61 60,61 62,61 63,61 65,61 66,61 67,61 68,61 69,62 46,62 47,62 54,62 56,62 57,62 59,62 60,62 62,62 63,62 65,62 66,62 67,62 68,62 69,63 46,63 47,63 54,63 56,63 57,63 59,63 60,63 62,63 63,63 65,63 66,63 67,63 68,63 69,65 66,67 46,67 47,67 54,67 56,67 57,67 59,67 60,67 62,67 63,67 65,67 66,67 67,67 68,67 69,68 69,7 9,71 100,71 72,71 80,71 83,71 85,71 86,71 87,71 89,71 90,71 91,71 92,71 93,71 95,71 96,71 97,71 99,73 100,73 80,73 85,73 87,73 89,73 91,73 97,73 99,74 100,74 75,74 80,74 83,74 85,74 86,74 87,74 89,74 90,74 91,74 92,74 93,74 95,74 96,74 97,74 99,75 100,75 80,75 83,75 85,75 86,75 87,75 89,75 90,75 91,75 92,75 93,75 95,75 96,75 97,75 99,8 9,82 100,82 80,82 83,82 85,82 86,82 87,82 89,82 90,82 91,82 92,82 93,82 95,82 96,82 97,82 99,83 100,83 80,83 83,83 85,83 86,83 87,83 89,83 90,83 91,83 92,83 93,83 95,83 96,83 97,83 99,85 100,85 80,85 87,85 89,85 91,85 99,86 100,86 80,86 83,86 85,86 86,86 87,86 89,86 90,86 91,86 92,86 93,86 95,86 96,86 97,86 99,87 100,87 80,87 89,87 91,87 99,89 100,89 91,89 99,91 100,92 100,92 93,92 95,92 96,92 97,92 99,95 100,96 100,96 95,97 100,97 99,99 100</t>
+  </si>
+  <si>
+    <t>stmt s1,s2,s3; variable v1;</t>
+  </si>
+  <si>
+    <t>Select s1 such that Uses(s1,v1) and Modifies(s1,v1) and Parent(s1,s2) and Follows(s2,s3)</t>
+  </si>
+  <si>
+    <t>4 clauses</t>
+  </si>
+  <si>
+    <t>stmt s1,s2,s3,s4; variable v1;</t>
+  </si>
+  <si>
+    <t>Select s1 such that Uses(s1,v1) and Modifies(s1,v1) and Parent(s1,s2) and Follows(s3,s4)</t>
+  </si>
+  <si>
+    <t>3-1 clauses</t>
+  </si>
+  <si>
+    <t>stmt s1,s2,s3,s4; variable v1,v2;</t>
+  </si>
+  <si>
+    <t>Select s1 such that Uses(s1,v1) and Modifies(s2,v2) and Parent(s1,s3) and Follows(s2,s4)</t>
+  </si>
+  <si>
+    <t>2-2 clauses</t>
+  </si>
+  <si>
+    <t>stmt s1,s2,s3,s4,s5; variable v1;</t>
+  </si>
+  <si>
+    <t>Select s1 such that Uses(s1,v1) and Modifies(s1,v1) and Parent(s2,s3) and Follows(s4,s5)</t>
+  </si>
+  <si>
+    <t>2-1-1 clauses</t>
+  </si>
+  <si>
+    <t>stmt s1,s2,s3,s4,s5,s6; variable v1,v2;</t>
+  </si>
+  <si>
+    <t>Select s1 such that Uses(s1,v1) and Modifies(s2,v2) and Parent(s3,s4) and Follows(s5,s6)</t>
+  </si>
+  <si>
+    <t>1-1-1-1 clauses</t>
+  </si>
+  <si>
+    <t>Select &lt;s1,s2&gt; such that Uses(s1,v1) and Modifies(s1,v1) and Parent(s1,s2) and Follows(s3,s4)</t>
+  </si>
+  <si>
+    <t>3-1 clauses 2 tuple</t>
+  </si>
+  <si>
+    <t>Select &lt;s1,s2,s3&gt; such that Uses(s1,v1) and Modifies(s1,v1) and Parent(s1,s2) and Follows(s3,s4)</t>
+  </si>
+  <si>
+    <t>3-1 clauses 3 tuple</t>
+  </si>
+  <si>
+    <t>Select &lt;s1,s2,s3,s4&gt; such that Uses(s1,v1) and Modifies(s1,v1) and Parent(s1,s2) and Follows(s3,s4)</t>
+  </si>
+  <si>
+    <t>3-1 clauses 4 tuple</t>
+  </si>
+  <si>
+    <t>Select &lt;s1,s2,s3,s4,v1&gt; such that Uses(s1,v1) and Modifies(s1,v1) and Parent(s1,s2) and Follows(s3,s4)</t>
+  </si>
+  <si>
+    <t>3-1 clauses 5 tuple</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stmt s1,s2,s3,s4,s5; </t>
+  </si>
+  <si>
+    <t>Select s1 such that Follows*(s1,s2) and Parent*(s2,s3) and Next*(s4,s5) and Affects*(s5,s6)</t>
+  </si>
+  <si>
+    <t>single tuple</t>
+  </si>
+  <si>
+    <t>Select &lt;s1,s2&gt; such that Follows*(s1,s2) and Parent*(s2,s3) and Next*(s4,s5) and Affects*(s5,s6)</t>
+  </si>
+  <si>
+    <t>double tuple</t>
+  </si>
+  <si>
+    <t>Select &lt;s1,s2,s3&gt; such that Follows*(s1,s2) and Parent*(s2,s3) and Next*(s4,s5) and Affects*(s5,s6)</t>
+  </si>
+  <si>
+    <t>triple tuple</t>
+  </si>
+  <si>
+    <t>Select &lt;s1,s2,s3,s4&gt; such that Follows*(s1,s2) and Parent*(s2,s3) and Next*(s4,s5) and Affects*(s5,s6)</t>
+  </si>
+  <si>
+    <t>four tuple</t>
+  </si>
+  <si>
+    <t>stmt s1,s2,s3,s4,s5,s6; variable v1;</t>
+  </si>
+  <si>
+    <t>Select s1 such that Follows*(s1,s2) and Parent*(s2,s3) and Next*(s4,s5) and Affects*(s5,s6) and Uses(s5,v1) and Modifies(s6,v1)</t>
+  </si>
+  <si>
+    <t>Select &lt;s1,s2&gt; such that Follows*(s1,s2) and Parent*(s2,s3) and Next*(s4,s5) and Affects*(s5,s6) and Uses(s5,v1) and Modifies(s6,v1)</t>
+  </si>
+  <si>
+    <t>Select &lt;s1,s2,s3&gt; such that Follows*(s1,s2) and Parent*(s2,s3) and Next*(s4,s5) and Affects*(s5,s6) and Uses(s5,v1) and Modifies(s6,v1)</t>
+  </si>
+  <si>
+    <t>Select &lt;s1,s2,s3,s4&gt; such that Follows*(s1,s2) and Parent*(s2,s3) and Next*(s4,s5) and Affects*(s5,s6) and Uses(s5,v1) and Modifies(s6,v1)</t>
+  </si>
+  <si>
+    <t>Select &lt;s1,s2,s3,s4,s5&gt; such that Follows*(s1,s2) and Parent*(s2,s3) and Next*(s4,s5) and Affects*(s5,s6) and Uses(s5,v1) and Modifies(s6,v1)</t>
+  </si>
+  <si>
+    <t>five tuple</t>
+  </si>
+  <si>
+    <t>Select &lt;s1,s2,s3,s4,s5,s6&gt; such that Follows*(s1,s2) and Parent*(s2,s3) and Next*(s4,s5) and Affects*(s5,s6) and Uses(s5,v1) and Modifies(s6,v1)</t>
+  </si>
+  <si>
+    <t>six tuple</t>
   </si>
 </sst>
 </file>
@@ -507,7 +630,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -534,6 +657,13 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1640,7 +1770,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDD5F34A-C32F-4F9E-A4EF-99404DBA2DE9}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
@@ -2094,12 +2224,321 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{937E14A3-23C2-45E6-9AB0-F9FD5DC183C0}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="34" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="66.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>3</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="10">
+        <v>4</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>5</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="10">
+        <v>6</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
+        <v>7</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="10">
+        <v>8</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
+        <v>10</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
+        <v>11</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
+        <v>12</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
+        <v>13</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
+        <v>14</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="10">
+        <v>15</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="10">
+        <v>16</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="10">
+        <v>17</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="10">
+        <v>18</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="10">
+        <v>19</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10" t="s">
+        <v>178</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>